<commit_message>
Add pivot source that uses an external connection
Pivot cache with external connection uses a driver to get data from some
kind of external storage. It can be database or workbook, web service...
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTable/Sources/PivotTable-AllSources-input.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTable/Sources/PivotTable-AllSources-input.xlsx
@@ -8,28 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\havli\source\repos\ClosedXML\ClosedXML.Tests\Resource\Other\PivotTable\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39F100C-E2D6-4D1D-970B-6328228E485D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C989D67D-7A97-4897-BBD0-9E58DC579EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10524" yWindow="4236" windowWidth="30960" windowHeight="12120" tabRatio="781" xr2:uid="{511D5D8F-76DE-4F5B-8C4B-E6E3D59723B0}"/>
+    <workbookView xWindow="5364" yWindow="2484" windowWidth="30960" windowHeight="12120" tabRatio="781" xr2:uid="{511D5D8F-76DE-4F5B-8C4B-E6E3D59723B0}"/>
   </bookViews>
   <sheets>
-    <sheet name="External - PT" sheetId="14" r:id="rId1"/>
-    <sheet name="Area Source" sheetId="1" r:id="rId2"/>
-    <sheet name="Area - PT" sheetId="8" r:id="rId3"/>
-    <sheet name="Table Source" sheetId="3" r:id="rId4"/>
-    <sheet name="Table - PT" sheetId="9" r:id="rId5"/>
-    <sheet name="Defined Name Source" sheetId="4" r:id="rId6"/>
-    <sheet name="Defined Name - PT" sheetId="10" r:id="rId7"/>
+    <sheet name="Connection - PT" sheetId="15" r:id="rId1"/>
+    <sheet name="External Workbook - PT" sheetId="14" r:id="rId2"/>
+    <sheet name="Area Source" sheetId="1" r:id="rId3"/>
+    <sheet name="Area - PT" sheetId="8" r:id="rId4"/>
+    <sheet name="Table Source" sheetId="3" r:id="rId5"/>
+    <sheet name="Table - PT" sheetId="9" r:id="rId6"/>
+    <sheet name="Defined Name Source" sheetId="4" r:id="rId7"/>
+    <sheet name="Defined Name - PT" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="AreaName">'Defined Name Source'!$B$2:$C$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="1" r:id="rId9"/>
-    <pivotCache cacheId="2" r:id="rId10"/>
-    <pivotCache cacheId="7" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
+    <pivotCache cacheId="2" r:id="rId11"/>
+    <pivotCache cacheId="3" r:id="rId12"/>
+    <pivotCache cacheId="5" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -48,8 +50,16 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{C541E7EC-78CE-4C7D-AB77-2894390EA7AF}" sourceFile="C:\Users\havli\source\repos\ClosedXML\ClosedXML.Tests\Resource\Other\PivotTable\Sources\PivotTable-AllSources-external-data.xlsx" keepAlive="1" name="PivotTable-AllSources-external-data" type="5" refreshedVersion="8" background="1">
+    <dbPr connection="Provider=Microsoft.ACE.OLEDB.12.0;User ID=Admin;Data Source=C:\Users\havli\source\repos\ClosedXML\ClosedXML.Tests\Resource\Other\PivotTable\Sources\PivotTable-AllSources-external-data.xlsx;Mode=Share Deny Write;Extended Properties=&quot;HDR=YES;&quot;;Jet OLEDB:System database=&quot;&quot;;Jet OLEDB:Registry Path=&quot;&quot;;Jet OLEDB:Engine Type=37;Jet OLEDB:Database Locking Mode=0;Jet OLEDB:Global Partial Bulk Ops=2;Jet OLEDB:Global Bulk Transactions=1;Jet OLEDB:New Database Password=&quot;&quot;;Jet OLEDB:Create System Database=False;Jet OLEDB:Encrypt Database=False;Jet OLEDB:Don't Copy Locale on Compact=False;Jet OLEDB:Compact Without Replica Repair=False;Jet OLEDB:SFP=False;Jet OLEDB:Support Complex Data=False;Jet OLEDB:Bypass UserInfo Validation=False;Jet OLEDB:Limited DB Caching=False;Jet OLEDB:Bypass ChoiceField Validation=False" command="Sheet1$" commandType="3"/>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -58,6 +68,21 @@
   </si>
   <si>
     <t>Cake</t>
+  </si>
+  <si>
+    <t>Pivot table that is using a connection to another workbook as a source of pivot cache. Connection uses absolute path, so it is necessary to update the path (Pivot Table Analyze - Change Data Source - Connection Properties - Definition).</t>
+  </si>
+  <si>
+    <t>Pivot table that uses area in 'Area Source' sheet as a source of data for the pivot cache.</t>
+  </si>
+  <si>
+    <t>Pivot table that uses external workbook reference as a source of data for the pivot cache.</t>
+  </si>
+  <si>
+    <t>Pivot table that uses a table named 'Table1' as a source of data for the pivot cache.</t>
+  </si>
+  <si>
+    <t>Pivot table that uses a defined name 'AreaName' as a source of data for the pivot cache.</t>
   </si>
 </sst>
 </file>
@@ -315,6 +340,31 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jan Havlíček" refreshedDate="45640.820318865743" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{08AFD5F3-EF3C-4277-9EC0-BC5F6E36BD65}">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="2">
+    <cacheField name="Name" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Cake"/>
+        <s v="Muffin"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Value" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="15" maxValue="16" count="2">
+        <n v="15"/>
+        <n v="16"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
@@ -355,8 +405,21 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="2">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D4D1264-DB58-4739-9865-48D4C248B3E1}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8B1473DA-4617-411E-B5E1-4F030EF43EB3}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="2">
     <pivotField showAll="0"/>
@@ -375,6 +438,25 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D4D1264-DB58-4739-9865-48D4C248B3E1}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="2">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{45F738BB-659D-4398-9BF8-4EF831A42BD4}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="2">
@@ -393,7 +475,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2B56FD51-7F09-4B25-B8A9-43A4A15B4CB4}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="2">
@@ -412,7 +494,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48B2550D-5C8A-4228-91A6-93B51A985389}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="2">
@@ -738,15 +820,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF7487B-601B-4CF1-83DA-637CE4ACBFAA}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157D16F0-CB70-40FE-8801-5E78DDAC6F12}">
-  <dimension ref="A3:C20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
@@ -842,7 +1037,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B95AC8F-0A2B-4305-8907-61BCB849A9DA}">
   <dimension ref="D3:E4"/>
   <sheetViews>
@@ -871,16 +1066,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF5682F4-C374-4D89-9ECF-B07973C4759C}">
-  <dimension ref="A3:C20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
@@ -976,7 +1174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96ED509-A698-481D-9229-D61A1CAE8227}">
   <dimension ref="B2:C3"/>
   <sheetViews>
@@ -1010,16 +1208,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{076680DD-97CF-4D98-B4D1-7E5361715DFA}">
-  <dimension ref="A3:C20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
@@ -1115,7 +1316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388DAB8D-43FF-4D7B-9586-E2AB978B4CFD}">
   <dimension ref="B2:C3"/>
   <sheetViews>
@@ -1146,16 +1347,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B5D2A0-EF2B-4557-801E-486063C03CDD}">
-  <dimension ref="A3:C20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>

</xml_diff>

<commit_message>
Add Scenario source load/save
Added the pivot cache with source to the test.
The actual pivot table in the output workbook is missing data and complains,
but the source is correct and doesn't throw on refresh.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTable/Sources/PivotTable-AllSources-input.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTable/Sources/PivotTable-AllSources-input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\havli\source\repos\ClosedXML\ClosedXML.Tests\Resource\Other\PivotTable\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C989D67D-7A97-4897-BBD0-9E58DC579EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C103D15-3D13-4E6D-8F54-B3C22D3DC05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5364" yWindow="2484" windowWidth="30960" windowHeight="12120" tabRatio="781" xr2:uid="{511D5D8F-76DE-4F5B-8C4B-E6E3D59723B0}"/>
+    <workbookView xWindow="5364" yWindow="2484" windowWidth="30960" windowHeight="12120" tabRatio="781" firstSheet="1" activeTab="9" xr2:uid="{511D5D8F-76DE-4F5B-8C4B-E6E3D59723B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Connection - PT" sheetId="15" r:id="rId1"/>
@@ -21,17 +21,20 @@
     <sheet name="Table - PT" sheetId="9" r:id="rId6"/>
     <sheet name="Defined Name Source" sheetId="4" r:id="rId7"/>
     <sheet name="Defined Name - PT" sheetId="10" r:id="rId8"/>
+    <sheet name="Scenario" sheetId="16" r:id="rId9"/>
+    <sheet name="Scenario PivotTable" sheetId="17" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="AreaName">'Defined Name Source'!$B$2:$C$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId9"/>
-    <pivotCache cacheId="1" r:id="rId10"/>
-    <pivotCache cacheId="2" r:id="rId11"/>
-    <pivotCache cacheId="3" r:id="rId12"/>
-    <pivotCache cacheId="5" r:id="rId13"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
+    <pivotCache cacheId="2" r:id="rId13"/>
+    <pivotCache cacheId="3" r:id="rId14"/>
+    <pivotCache cacheId="4" r:id="rId15"/>
+    <pivotCache cacheId="5" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -59,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -83,6 +86,30 @@
   </si>
   <si>
     <t>Pivot table that uses a defined name 'AreaName' as a source of data for the pivot cache.</t>
+  </si>
+  <si>
+    <t>Pie</t>
+  </si>
+  <si>
+    <t>Total with tax</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>$B$5</t>
+  </si>
+  <si>
+    <t>Expensive</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>$B$2:$B$3 by</t>
+  </si>
+  <si>
+    <t>(All)</t>
   </si>
 </sst>
 </file>
@@ -228,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -239,6 +266,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,6 +397,36 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Jan Havlíček" refreshedDate="45640.931218171296" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{9BD42A5F-5A0C-417E-AEDF-DBA25499EC16}">
+  <cacheSource type="scenario"/>
+  <cacheFields count="3">
+    <cacheField name="$B$2:$B$3" numFmtId="0">
+      <sharedItems containsNonDate="0" count="2">
+        <s v="Original"/>
+        <s v="Expensive"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="$B$2:$B$3 by" numFmtId="0">
+      <sharedItems containsNonDate="0" count="1">
+        <s v="Jan Havlíček"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="res $B$5" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsString="0" containsNumber="1" minValue="30.25" maxValue="151.25" count="2">
+        <n v="30.25"/>
+        <n v="151.25"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
@@ -419,7 +481,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8B1473DA-4617-411E-B5E1-4F030EF43EB3}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8B1473DA-4617-411E-B5E1-4F030EF43EB3}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="2">
     <pivotField showAll="0"/>
@@ -501,6 +563,56 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
   </pivotFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CD5C9CDA-F86E-415A-B8D1-75DC461E852E}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="A3:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="$B$5" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -823,7 +935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF7487B-601B-4CF1-83DA-637CE4ACBFAA}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -921,6 +1033,55 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC5C1F4-162A-4495-BD7F-5FACEE21B0F8}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="12">
+        <v>151.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="12">
+        <v>30.25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1455,4 +1616,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB5288C-1114-45E0-9330-28F95507E82B}">
+  <dimension ref="A2:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <f>(B2+B3)*1.21</f>
+        <v>30.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <scenarios current="0" show="0" sqref="B5">
+    <scenario name="Original" locked="1" count="2" user="Jan Havlíček" comment="Created by Jan Havlíček on 12/14/2024">
+      <inputCells r="B2" val="10"/>
+      <inputCells r="B3" val="15"/>
+    </scenario>
+    <scenario name="Expensive" locked="1" count="2" user="Jan Havlíček" comment="Created by Jan Havlíček on 12/14/2024">
+      <inputCells r="B2" val="50"/>
+      <inputCells r="B3" val="75"/>
+    </scenario>
+  </scenarios>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add load/store for consolidate pivot source
Consolidate pivot table combines several areas to into one source. It is
limited, e.g. value can only be numbers (I think).

Consolidate pivot source is basically a legacy feature, but still
available through Alt+D,P keyboard shortcut.

This adds the sturctures for loading the XML and saving the XML. The end
goal is full representation of OOXML in the ClosedXML.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTable/Sources/PivotTable-AllSources-input.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTable/Sources/PivotTable-AllSources-input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\havli\source\repos\ClosedXML\ClosedXML.Tests\Resource\Other\PivotTable\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C103D15-3D13-4E6D-8F54-B3C22D3DC05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538143E2-3B8F-4339-B8C8-D3C86837AED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5364" yWindow="2484" windowWidth="30960" windowHeight="12120" tabRatio="781" firstSheet="1" activeTab="9" xr2:uid="{511D5D8F-76DE-4F5B-8C4B-E6E3D59723B0}"/>
+    <workbookView xWindow="5364" yWindow="2484" windowWidth="30960" windowHeight="12120" tabRatio="781" firstSheet="3" activeTab="11" xr2:uid="{511D5D8F-76DE-4F5B-8C4B-E6E3D59723B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Connection - PT" sheetId="15" r:id="rId1"/>
@@ -22,19 +22,22 @@
     <sheet name="Defined Name Source" sheetId="4" r:id="rId7"/>
     <sheet name="Defined Name - PT" sheetId="10" r:id="rId8"/>
     <sheet name="Scenario" sheetId="16" r:id="rId9"/>
-    <sheet name="Scenario PivotTable" sheetId="17" r:id="rId10"/>
+    <sheet name="Scenario - PT" sheetId="17" r:id="rId10"/>
+    <sheet name="Consolidate" sheetId="18" r:id="rId11"/>
+    <sheet name="Consolidate - PT" sheetId="19" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="AreaName">'Defined Name Source'!$B$2:$C$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId11"/>
-    <pivotCache cacheId="1" r:id="rId12"/>
-    <pivotCache cacheId="2" r:id="rId13"/>
-    <pivotCache cacheId="3" r:id="rId14"/>
-    <pivotCache cacheId="4" r:id="rId15"/>
-    <pivotCache cacheId="5" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId13"/>
+    <pivotCache cacheId="1" r:id="rId14"/>
+    <pivotCache cacheId="2" r:id="rId15"/>
+    <pivotCache cacheId="3" r:id="rId16"/>
+    <pivotCache cacheId="4" r:id="rId17"/>
+    <pivotCache cacheId="5" r:id="rId18"/>
+    <pivotCache cacheId="6" r:id="rId19"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -62,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -110,6 +113,27 @@
   </si>
   <si>
     <t>(All)</t>
+  </si>
+  <si>
+    <t>Muffin</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>Sum of Value</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Page1</t>
+  </si>
+  <si>
+    <t>Page2</t>
   </si>
 </sst>
 </file>
@@ -427,6 +451,67 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jan Havlíček" refreshedDate="45641.123992361114" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="3" xr:uid="{C4D000D4-C547-41E9-B0B9-2D56DCDF4F13}">
+  <cacheSource type="consolidation">
+    <consolidation autoPage="0">
+      <pages count="2">
+        <page count="2">
+          <pageItem name="Cakes"/>
+          <pageItem name="Taxes"/>
+        </page>
+        <page count="2">
+          <pageItem name="Cakes"/>
+          <pageItem name="Tax1"/>
+        </page>
+      </pages>
+      <rangeSets count="2">
+        <rangeSet i1="0" i2="0" ref="A1:B3" sheet="Consolidate"/>
+        <rangeSet i1="1" i2="1" ref="D1:E2" sheet="Consolidate"/>
+      </rangeSets>
+    </consolidation>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="Row" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Cake"/>
+        <s v="Muffin"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Column" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Value"/>
+        <s v="Tax"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Value" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.21" maxValue="25" count="3">
+        <n v="25"/>
+        <n v="17"/>
+        <n v="1.21"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Page1" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Cakes"/>
+        <s v="Taxes"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Page2" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Cakes"/>
+        <s v="Tax1"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
@@ -474,6 +559,32 @@
     <x v="0"/>
   </r>
   <r>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="3">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
   </r>
@@ -612,6 +723,87 @@
   </pageFields>
   <dataFields count="1">
     <dataField name="$B$5" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FEEAA086-841A-475E-91D3-9CEF17819C08}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:D8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="3" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1043,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC5C1F4-162A-4495-BD7F-5FACEE21B0F8}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1071,7 +1263,7 @@
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4">
         <v>151.25</v>
       </c>
     </row>
@@ -1079,8 +1271,158 @@
       <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5">
         <v>30.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F178DE-BBB7-489C-9228-24C8800DF773}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4D42AF-FE37-4EC3-9D02-CE3B6F12778F}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1.21</v>
+      </c>
+      <c r="C6" s="12">
+        <v>25</v>
+      </c>
+      <c r="D6" s="12">
+        <v>26.21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12">
+        <v>17</v>
+      </c>
+      <c r="D7" s="12">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1.21</v>
+      </c>
+      <c r="C8" s="12">
+        <v>42</v>
+      </c>
+      <c r="D8" s="12">
+        <v>43.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>